<commit_message>
derniere modification graphique et tableaux
</commit_message>
<xml_diff>
--- a/Streamlit/assets/Les datasets/dataset_comparison.xlsx
+++ b/Streamlit/assets/Les datasets/dataset_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repository\datasciencetest_reco_plante\Streamlit\assets\Les datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C7BDAE-FFE4-4AE7-81AE-49B46E148949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B9B035-B197-49DD-9F84-601AF7BF9504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{3B820FF9-CF19-443E-ABFA-59F6CC72F095}"/>
+    <workbookView xWindow="28680" yWindow="3630" windowWidth="29040" windowHeight="15720" xr2:uid="{3B820FF9-CF19-443E-ABFA-59F6CC72F095}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>PlantVillage</t>
   </si>
@@ -62,27 +62,18 @@
     <t>14 espèces de plantes</t>
   </si>
   <si>
-    <t>38 classes de maladies sur plusieurs espèces</t>
-  </si>
-  <si>
     <t>Nombre de maladies</t>
   </si>
   <si>
     <t>26 maladies (avec healthy classes)</t>
   </si>
   <si>
-    <t>~120 maladies (certaines classes rares)</t>
-  </si>
-  <si>
     <t>Type d’image</t>
   </si>
   <si>
     <t>Images avec des fonds unis</t>
   </si>
   <si>
-    <t xml:space="preserve">Images prises en milieu naturel  </t>
-  </si>
-  <si>
     <t>Annotation</t>
   </si>
   <si>
@@ -92,9 +83,6 @@
     <t>Espèce + maladie</t>
   </si>
   <si>
-    <t>Espèce + maladie + conditions environnementales</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
@@ -110,63 +98,22 @@
     <t>Accessibilité</t>
   </si>
   <si>
-    <t>Ouvert (Kaggle, GitHub)</t>
-  </si>
-  <si>
     <t>Ouvert (Kaggle)</t>
   </si>
   <si>
-    <t>Ouvert (Google Dataset Search, Zenodo, etc.)</t>
-  </si>
-  <si>
     <t>Caractéristiques</t>
   </si>
   <si>
-    <t>plus de 60 espèces de plantes</t>
-  </si>
-  <si>
-    <t>plus de 50 maladies (certaines plantes avec plusieurs maladies)</t>
-  </si>
-  <si>
     <t>nombre de classes</t>
   </si>
   <si>
     <t>38 classes (espèce + maladie / healthy)</t>
   </si>
   <si>
-    <r>
-      <t>~54,000 images</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>38 classes (espèce + maladie ou healthy)</t>
-    </r>
-  </si>
-  <si>
     <t>Commentaire</t>
   </si>
   <si>
     <t>Une redistribution / réorganisation de PlantVillage sur Kaggle (organisation de fichiers différente, sans ajout de nouvelles espèces, maladies ou informations visuelles)</t>
-  </si>
-  <si>
-    <r>
-      <t>Images variées</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, prises sur le terrain</t>
-    </r>
   </si>
   <si>
     <t>Une version augmentée artificiellement de PlantVillage (Images générées par rotations, flips, zooms)</t>
@@ -179,7 +126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,26 +148,12 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
+      <color theme="8" tint="0.39997558519241921"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="8" tint="0.39997558519241921"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -245,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -373,26 +306,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF00B0F0"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF00B0F0"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF00B0F0"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF00B0F0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -406,13 +324,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -421,37 +351,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -791,20 +694,20 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="4" max="4" width="28.81640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -816,130 +719,130 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="23" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="23" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="C6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="23" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="D7" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="19" t="s">
+      <c r="C9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="96" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="B10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D10" s="7" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="80.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrections partie desc datasets
</commit_message>
<xml_diff>
--- a/Streamlit/assets/Les datasets/dataset_comparison.xlsx
+++ b/Streamlit/assets/Les datasets/dataset_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repository\datasciencetest_reco_plante\Streamlit\assets\Les datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B9B035-B197-49DD-9F84-601AF7BF9504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2371E1-A311-41CA-9958-6E62905BDCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="3630" windowWidth="29040" windowHeight="15720" xr2:uid="{3B820FF9-CF19-443E-ABFA-59F6CC72F095}"/>
+    <workbookView xWindow="13180" yWindow="4810" windowWidth="21600" windowHeight="11180" xr2:uid="{3B820FF9-CF19-443E-ABFA-59F6CC72F095}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>PlantVillage</t>
   </si>
@@ -80,21 +80,12 @@
     <t>Espèce + maladie + healthy</t>
   </si>
   <si>
-    <t>Espèce + maladie</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
-    <t>JPG / PNG</t>
-  </si>
-  <si>
     <t>JPG</t>
   </si>
   <si>
-    <t>JPG / JPEG / PNG</t>
-  </si>
-  <si>
     <t>Accessibilité</t>
   </si>
   <si>
@@ -104,12 +95,6 @@
     <t>Caractéristiques</t>
   </si>
   <si>
-    <t>nombre de classes</t>
-  </si>
-  <si>
-    <t>38 classes (espèce + maladie / healthy)</t>
-  </si>
-  <si>
     <t>Commentaire</t>
   </si>
   <si>
@@ -120,6 +105,12 @@
   </si>
   <si>
     <t>Le dataset de référence en détection des maladies des plantes, créé dans un cadre contrôlé</t>
+  </si>
+  <si>
+    <t>~54 000 images uniques (≈163 000 fichiers avec color / grayscale / segmented)</t>
+  </si>
+  <si>
+    <t>JPG (majoritaire), PNG/JPEG (résiduels)</t>
   </si>
 </sst>
 </file>
@@ -310,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -352,9 +343,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -691,23 +679,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7D3492-221B-4771-9BEA-C588526E2089}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -719,12 +707,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="46" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>4</v>
@@ -733,7 +721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="23" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -747,7 +735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="23" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -761,88 +749,74 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:4" ht="23" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="23" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="23" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="96" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>26</v>
+      <c r="D9" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>